<commit_message>
combined keyword search and wildcard into one,  where wildcard need identifier
</commit_message>
<xml_diff>
--- a/download_table/output.xlsx
+++ b/download_table/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,91 +453,211 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>clinica%</t>
+          <t>a%</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/ideas-grants</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/postgraduate-scholarships</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>clinica%</t>
+          <t>a%</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/clinical-trials-and-cohort-studies-grants</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/partnership-projects</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>clinica%</t>
+          <t>a%</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/cre</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/development-grants</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>clinica%</t>
+          <t>a%</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/manage-your-grant</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/cre</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>clinica%</t>
+          <t>a%</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/ideas-grants#Funding%20Partners</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/ideas-grants</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>clinica%</t>
+          <t>a%</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/targeted-calls/nhmrc-e-asia-joint-research-program-grants</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/targeted-calls</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>clinica%</t>
+          <t>a%</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/investigator-grants</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>a%</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/synergy-grants</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>a%</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/clinical-trials-and-cohort-studies-grants</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>a%</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/manage-your-grant</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>a%</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/targeted-calls/eucrg</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>a%</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/targeted-calls/nhmrc-e-asia-joint-research-program-grants</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>a%</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/ideas-grants#Funding%20Partners</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>a%</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/targeted-calls/nhmrc-collaborations-in-health-services-research</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>clinica%</t>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>a%</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/targeted-calls/nhmrc-amed-2024-aspire</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>a%</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/targeted-calls/2024-nhmrc-cihr-ccna</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>a%</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/targeted-calls/nhmrc-gacd-funding-call</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>a%</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
uom sign links excel download table added
</commit_message>
<xml_diff>
--- a/download_table/output.xlsx
+++ b/download_table/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,6 +441,11 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>source_link</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>associated_text</t>
         </is>
       </c>
@@ -448,216 +453,731 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc</t>
+          <t>https://gateway.research.unimelb.edu.au/resources/ip-and-commercialisation</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>a%</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Go to the Research Gateway</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/postgraduate-scholarships</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/international/international-codes-and-contacts%20</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>a%</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/international</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>International Codes and Contacts</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/partnership-projects</t>
+          <t>http://www.eventbrite.com.au/o/research-innovation-amp-commercialisation-626087145</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>a%</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/resources</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>EventBrite</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/development-grants</t>
+          <t>https://gateway.research.unimelb.edu.au/services/research-innovation-and-commercialisation/micg</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>a%</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/international</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>relevant grants team</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/cre</t>
+          <t>https://gateway.research.unimelb.edu.au/__data/assets/file/0008/3236219/Request-to-change-Departments.msg</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>a%</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/manage-your-grant</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Themis TR1D form</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/ideas-grants</t>
+          <t>http://www.arc.gov.au/arc-centres-excellence%20</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>a%</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/coe</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>ARC Centres of Excellence</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/targeted-calls</t>
+          <t>https://gateway.research.unimelb.edu.au/__data/assets/file/0018/3236220/Request-to-share-funding-between-University-of-Melbourne-departments-TR1F.msg</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>a%</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/manage-your-grant</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Themis TR1F form</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/investigator-grants</t>
+          <t>https://healthandmedicalresearch.gov.au/images/help/NHMRC%20Sapphire%20MFA%20guide_HMR.pdf</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>a%</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/synergy-grants</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>NHMRC guide</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>https://staff.unimelb.edu.au/mdhs/research-development/research-collaboration-and-funding/grant-mentoring?_ga=2.207383891.1926808974.1707085361-5606f16a62243141946ac55ffe06e6048610a76b42147e009b562ba4af819daa</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/synergy-grants</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>a%</t>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>MDHS Townhall videos</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/clinical-trials-and-cohort-studies-grants</t>
+          <t>http://musse.unimelb.edu.au/october-12-97/woodward-medals-honour-history-and-science</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>a%</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/researcher-development-schemes/woodward-medallists</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Article</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>https://gateway.research.unimelb.edu.au/resources/ethics-and-integrity/research-integrity/research-integrity-in-practice/conflict-of-interest</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/manage-your-grant</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>a%</t>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>here</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/targeted-calls/eucrg</t>
+          <t>https://staff.unimelb.edu.au/research/research-systems/research-themis-guides/grants,-contracts-and-submissions/create-a-grant-submission-record</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>a%</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/researcher-development-schemes/melbourne-indonesia-research-partnership-program</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Themis guide</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/targeted-calls/nhmrc-e-asia-joint-research-program-grants</t>
+          <t>http://musse.unimelb.edu.au/february-11-53/woodward-medallists-named</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>a%</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/researcher-development-schemes/woodward-medallists</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Article</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/ideas-grants#Funding%20Partners</t>
+          <t>http://blogs.unimelb.edu.au/researchnews/2011/12/19/woodward-medals/</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>a%</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/researcher-development-schemes/woodward-medallists</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Article</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/targeted-calls/nhmrc-collaborations-in-health-services-research</t>
+          <t>http://research.unimelb.edu.au/contact-us</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>a%</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/domestic</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>relevant grants team</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/targeted-calls/nhmrc-amed-2024-aspire</t>
+          <t>https://www.manchester.ac.uk/collaborate/worldwide/collaborations/manchester-melbourne-research-fund/</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>a%</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/researcher-development-schemes/university-of-melbourne-university-of-manchester-research-fund</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Manchester-Melbourne Research Fund scheme website</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/targeted-calls/2024-nhmrc-cihr-ccna</t>
+          <t>https://fbe-research.smartygrants.com.au/DE25</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>a%</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/researcher-development-schemes/establishment-grants-decra</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Smartygrants</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/targeted-calls/nhmrc-gacd-funding-call</t>
+          <t>http://blogs.unimelb.edu.au/musse/?p=466</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>a%</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/researcher-development-schemes/woodward-medallists</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Article</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>https://staff.unimelb.edu.au/research/grants/materials-past-seminars/us-grant-accelerator-program-workshops</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/international/department-of-defense-dod</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>https://staff.unimelb.edu.au/research/grants/materials-past-seminars/us-grant-accelerator-program-workshops</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>https://library.unimelb.edu.au/openscholarship/open-access-publishing</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/researcher-development-schemes/the-carlo-and-rita-giugni-ecr-grant-for-aged-care-research</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>https://library.unimelb.edu.au/openscholarship/open-access-publishing;</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>https://vimeo.com/447312256/4c26b49d1a</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/early-career-industry-fellowship</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/uc?export=download&amp;id=1XDQD4_K65J0Ur4nRWi-1UbTlh_EdPzC1</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/researcher-development-schemes/invertebrate-management-research-seed-funding-scheme</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>[Errno 22] Invalid argument: 'downloads\\uc?export=download&amp;id=1XDQD4_K65J0Ur4nRWi-1UbTlh_EdPzC1'</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>https://vimeo.com/780543000</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/discovery-indigenous</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>video</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>https://gateway.research.unimelb.edu.au/resources/outputs/research-outputs-support</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/discovery-indigenous</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>UoM Manage your research outputs</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>https://www.eventbrite.com.au/e/491443991207</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/mrff/EMCR-Workshop-series-MRFF</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Please register your interest in the series</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>https://portal.bihealth.de/portal/</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/researcher-development-schemes/BUA</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>https://portal.bihealth.de/portal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>http://www.business.vic.gov.au/support-for-your-business/future-industries/sectorgrowth</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/mi/victorian-future-industries-fund</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Sector Growth Program</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>http://www.business.vic.gov.au/__data/assets/pdf_file/0007/1272364/Sector-Growth-Fact-Sheet.pdf</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/mi/victorian-future-industries-fund</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sector Growth Program Fact Sheet </t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>http://www.business.vic.gov.au/__data/assets/pdf_file/0004/1253245/NEJF-Application-Guidelines-21-Jan.pdf</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/mi/victorian-future-industries-fund</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>New Energy Jobs Fund Guidelines</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>http://www.business.vic.gov.au/__data/assets/pdf_file/0006/1272363/Sector-Growth-Program-Guidelines.pdf</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/mi/victorian-future-industries-fund</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Sector Growth Program Guidelines</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>http://www.business.vic.gov.au/__data/assets/pdf_file/0007/1242916/9348-DEDJTR-VFI-Fundsheet_NEW-ENERGY_GREEN-PROOF-v11.pdf</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/mi/victorian-future-industries-fund</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Energy Jobs Fund Fact Sheet </t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>http://www.business.vic.gov.au/support-for-your-business/future-industries/future-industries-manufacturing-program</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/mi/victorian-future-industries-fund</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Future Industries Manufacturing Program</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>http://www.arc.gov.au/important-dates</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/manage-your-grant</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Important Dates webpage</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>http://www.business.vic.gov.au/__data/assets/pdf_file/0006/1219335/Future-IndustriesI-Manufacturing-Program-Guidelines-.pdf</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/mi/victorian-future-industries-fund</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Manufacturing Program Guidelines</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>http://www.business.vic.gov.au/__data/assets/pdf_file/0009/1219356/Future-Industries-Manufacturing-Program-Fact-Sheet.pdf</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/mi/victorian-future-industries-fund</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Manufacturing Program Fact Sheet</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>https://staff.unimelb.edu.au/research/research-systems/research-themis-guides/change-to-agreement-records-forms</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/manage-your-grant</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>website</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>https://www.arc.gov.au/grants/grant-administration</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/manage-your-grant</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>post-award variation</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>http://www.arc.gov.au/funding-agreement</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/manage-your-grant</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>ARC Funding/Grant Agreement</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>http://research.unimelb.edu.au/contact-us/university-wide-contacts</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/arc/manage-your-grant</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>RIC staff</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>https://wellcome.ac.uk/funding/innovator-awards-digital-technologies</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/international/wellcome-trust</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>https://wellcome.ac.uk/funding/innovator-awards-digital-technologies</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>https://www.nhmrc.gov.au/file/14279/download?token=aK5Kr_gZ</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/targeted-calls/eucrg</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Direct Research Costs</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>https://research.unimelb.edu.au/partner/technology-licensing/for-researchers/intellectual-property-for-researchers</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/international/international-codes-and-contacts</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Case-by-case</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>https://facultyandstaff.sgs.utoronto.ca/gfm/gfm-faqs</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/researcher-development-schemes/toronto-melbourne-irtg-call-for-proposals</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Full School of Graduate Studies (SGS) Graduate Faculty Membership</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
redirecting to a new link for result page
</commit_message>
<xml_diff>
--- a/download_table/output.xlsx
+++ b/download_table/output.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -425,7 +437,144 @@
     <col width="100" customWidth="1" min="2" max="2"/>
     <col width="50" customWidth="1" min="3" max="3"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>source_link</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>associated_text</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>https://healthandmedicalresearch.gov.au/images/help/NHMRC%20Sapphire%20MFA%20guide_HMR.pdf</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/synergy-grants</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>NHMRC guide</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>https://www.nhmrc.gov.au/file/18387/download?token=NBnWlQ8-</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/manage-your-grant</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>[Errno 22] Invalid argument: 'downloads\\download?token=NBnWlQ8-'</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>https://staff.unimelb.edu.au/mdhs/research-development/research-collaboration-and-funding/grant-mentoring?_ga=2.207383891.1926808974.1707085361-5606f16a62243141946ac55ffe06e6048610a76b42147e009b562ba4af819daa</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/synergy-grants</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>MDHS Townhall videos</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>https://gateway.research.unimelb.edu.au/__data/assets/file/0018/3236220/Request-to-share-funding-between-University-of-Melbourne-departments-TR1F.msg</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/manage-your-grant</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Themis TR1F form</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>https://gateway.research.unimelb.edu.au/__data/assets/file/0008/3236219/Request-to-change-Departments.msg</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/manage-your-grant</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Themis TR1D form</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>https://www.nhmrc.gov.au/file/14279/download?token=aK5Kr_gZ</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/targeted-calls/eucrg</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Direct Research Costs</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>https://gateway.research.unimelb.edu.au/resources/ethics-and-integrity/research-integrity/research-integrity-in-practice/conflict-of-interest</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/manage-your-grant</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>here</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add searching result redirection test
</commit_message>
<xml_diff>
--- a/download_table/output.xlsx
+++ b/download_table/output.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,144 +425,7 @@
     <col width="100" customWidth="1" min="2" max="2"/>
     <col width="50" customWidth="1" min="3" max="3"/>
   </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>url</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>source_link</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>associated_text</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>https://healthandmedicalresearch.gov.au/images/help/NHMRC%20Sapphire%20MFA%20guide_HMR.pdf</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/synergy-grants</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>NHMRC guide</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>https://www.nhmrc.gov.au/file/18387/download?token=NBnWlQ8-</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/manage-your-grant</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>[Errno 22] Invalid argument: 'downloads\\download?token=NBnWlQ8-'</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>https://staff.unimelb.edu.au/mdhs/research-development/research-collaboration-and-funding/grant-mentoring?_ga=2.207383891.1926808974.1707085361-5606f16a62243141946ac55ffe06e6048610a76b42147e009b562ba4af819daa</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/synergy-grants</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>MDHS Townhall videos</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>https://gateway.research.unimelb.edu.au/__data/assets/file/0018/3236220/Request-to-share-funding-between-University-of-Melbourne-departments-TR1F.msg</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/manage-your-grant</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Themis TR1F form</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>https://gateway.research.unimelb.edu.au/__data/assets/file/0008/3236219/Request-to-change-Departments.msg</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/manage-your-grant</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Themis TR1D form</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>https://www.nhmrc.gov.au/file/14279/download?token=aK5Kr_gZ</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/targeted-calls/eucrg</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Direct Research Costs</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>https://gateway.research.unimelb.edu.au/resources/ethics-and-integrity/research-integrity/research-integrity-in-practice/conflict-of-interest</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/manage-your-grant</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>here</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
push to switch branch
</commit_message>
<xml_diff>
--- a/download_table/output.xlsx
+++ b/download_table/output.xlsx
@@ -458,7 +458,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>a b c</t>
+          <t>for</t>
         </is>
       </c>
     </row>
@@ -470,7 +470,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>a b c</t>
+          <t>for</t>
         </is>
       </c>
     </row>
@@ -482,7 +482,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>a b c</t>
+          <t>FOR</t>
         </is>
       </c>
     </row>
@@ -494,7 +494,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>a b c</t>
+          <t>for</t>
         </is>
       </c>
     </row>
@@ -506,31 +506,31 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>a b c</t>
+          <t>for</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/international/international-codes-and-contacts</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/international/wellcome-trust</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>a b c</t>
+          <t>for</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/international/wellcome-trust</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/international/international-codes-and-contacts</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>a b c</t>
+          <t>for</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
revise logics of searching
</commit_message>
<xml_diff>
--- a/download_table/output.xlsx
+++ b/download_table/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,84 +453,108 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/international</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/domestic</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>a b c</t>
+          <t>Accepting and managing your funding</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/international/department-of-defense-dod</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/domestic/manage-your-grant</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>a b c</t>
+          <t>Accepting, and, funding, managing, your</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/international/national-institutes-of-health-scheme</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/domestic/cancer-council-victoria-grants-in-aid</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>a b c</t>
+          <t>Accepting, and, funding, managing, your</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/international/department-of-defense-dod/dod-agencies</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/domestic/vca-grants</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>a b c</t>
+          <t>Accepting, and, funding, managing, your</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/international/national-institutes-of-health-scheme/national-institutes-of-health</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/domestic/victorian-cancer-agency-grants2</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>a b c</t>
+          <t>Accepting, and, funding, managing, your</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/international/international-codes-and-contacts</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/domestic/schemes-for-international-collaboration</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>a b c</t>
+          <t>Accepting, and, funding, managing, your</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/international/wellcome-trust</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/domestic/westpac</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>a b c</t>
+          <t>Accepting, and, funding, managing, your</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/domestic/djpr-victorian-medical-research-acceleration-fund-vmraf-and-mrna-vmraf</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Accepting, and, funding, managing, your</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/domestic/mrna-vraf</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Accepting, and, funding, managing, your</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixbugs of sorting result
</commit_message>
<xml_diff>
--- a/download_table/output.xlsx
+++ b/download_table/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,108 +453,216 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/domestic</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/targeted-calls/nhmrc-e-asia-joint-research-program-grants</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Accepting and managing your funding</t>
+          <t>AEDTApplications</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/domestic/manage-your-grant</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/partnership-projects</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Accepting, and, funding, managing, your</t>
+          <t>ASAP</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/domestic/cancer-council-victoria-grants-in-aid</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/development-grants</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Accepting, and, funding, managing, your</t>
+          <t>ASAPRegister</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/domestic/vca-grants</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/ideas-grants</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Accepting, and, funding, managing, your</t>
+          <t>ASAPRegister</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/domestic/victorian-cancer-agency-grants2</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/ideas-grants#Funding%20Partners</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Accepting, and, funding, managing, your</t>
+          <t>ASAPRegister</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/domestic/schemes-for-international-collaboration</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/targeted-calls/nhmrc-gacd-funding-call</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Accepting, and, funding, managing, your</t>
+          <t>ASAPRegister</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/domestic/westpac</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Accepting, and, funding, managing, your</t>
+          <t>Accepting</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/domestic/djpr-victorian-medical-research-acceleration-fund-vmraf-and-mrna-vmraf</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/manage-your-grant</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Accepting, and, funding, managing, your</t>
+          <t>Accepting</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://sites.research.unimelb.edu.au/research-funding/domestic/mrna-vraf</t>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/targeted-calls/nhmrc-amed-2024-aspire</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Accepting, and, funding, managing, your</t>
+          <t>Adopting</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/targeted-calls/2024-nhmrc-cihr-ccna</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Aging</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/postgraduate-scholarships</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/targeted-calls/nhmrc-collaborations-in-health-services-research</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>August</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/targeted-calls</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Australian</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/cre</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>aims</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/synergy-grants</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>and</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/clinical-trials-and-cohort-studies-grants</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>and</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/investigator-grants</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>approvals,</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>https://sites.research.unimelb.edu.au/research-funding/nhmrc/targeted-calls/eucrg</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>available4</t>
         </is>
       </c>
     </row>

</xml_diff>